<commit_message>
Asignacion de Valores a los componentes pasivos de las tarjetas de Testeo. Actualziacion de las BOMs.
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/CIRULO_PANEL.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/CIRULO_PANEL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\TEAMDR~1\JRODRI~1\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3897AC7E-A242-4941-945B-6C8B320683BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6875AABC-DC56-4796-B49F-3396A56E6EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CIRULO PANEL" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Qty</t>
   </si>
@@ -71,9 +71,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>10K</t>
-  </si>
-  <si>
     <t>R40</t>
   </si>
   <si>
@@ -177,12 +174,18 @@
   </si>
   <si>
     <t>HISTORY</t>
+  </si>
+  <si>
+    <t>100n</t>
+  </si>
+  <si>
+    <t>Valor de Condensadores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -813,15 +816,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -833,6 +827,15 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -910,14 +913,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -955,7 +958,9 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{CFFEAB8C-9ABF-4404-A68A-FA64670E3401}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -968,22 +973,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla133" displayName="Tabla133" ref="A6:J18" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="10">
-  <autoFilter ref="A6:J18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla133" displayName="Tabla133" ref="A6:J18" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
+  <autoFilter ref="A6:J18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:J18">
     <sortCondition ref="D6:D18"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" name="Position" dataDxfId="9"/>
-    <tableColumn id="2" name="NEW" dataDxfId="8"/>
-    <tableColumn id="3" name="Qty" dataDxfId="7"/>
-    <tableColumn id="4" name="Part" dataDxfId="6"/>
-    <tableColumn id="5" name="Value" dataDxfId="5"/>
-    <tableColumn id="6" name="Device" dataDxfId="4"/>
-    <tableColumn id="7" name="Package" dataDxfId="3"/>
-    <tableColumn id="8" name="Unit Price" dataDxfId="2"/>
-    <tableColumn id="9" name="Extended Price" dataDxfId="1"/>
-    <tableColumn id="10" name="Link" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Position" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NEW" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Qty" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Part" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Value" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Device" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Package" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Unit Price" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Extended Price" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Link" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1278,18 +1283,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,26 +1315,26 @@
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="12">
-        <v>1</v>
+      <c r="A2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="9">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="27" x14ac:dyDescent="0.4">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="27" x14ac:dyDescent="0.4">
-      <c r="B4" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
+      <c r="B4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:10" ht="27" x14ac:dyDescent="0.4">
       <c r="B5" s="6"/>
@@ -1339,16 +1344,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>1</v>
@@ -1360,13 +1365,13 @@
         <v>3</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1384,7 +1389,7 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -1406,11 +1411,14 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1428,7 +1436,7 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
         <v>9</v>
@@ -1455,7 +1463,7 @@
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1470,16 +1478,16 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
         <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1497,7 +1505,7 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" t="s">
         <v>4</v>
@@ -1518,7 +1526,7 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
@@ -1539,7 +1547,7 @@
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
         <v>7</v>
@@ -1557,16 +1565,16 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1581,16 +1589,16 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
         <v>16</v>
       </c>
+      <c r="E16">
+        <v>220</v>
+      </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1605,16 +1613,16 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
         <v>21</v>
-      </c>
-      <c r="F17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" t="s">
-        <v>22</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1629,16 +1637,16 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
         <v>24</v>
-      </c>
-      <c r="F18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" t="s">
-        <v>25</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1656,11 +1664,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,48 +1677,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
-        <v>51</v>
+      <c r="A1" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>47</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="11">
         <v>44943</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11">
+        <v>44950</v>
+      </c>
+      <c r="C5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
+      <c r="B6" s="11"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
+      <c r="B7" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>